<commit_message>
Adicionando exercicio com tratamento de erro
</commit_message>
<xml_diff>
--- a/TestesMesa/Testes_de_Mesa.xlsx
+++ b/TestesMesa/Testes_de_Mesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Just Coding\JAVA\FATEC\LP1\TestesMesa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFABDBCD-655E-4CD5-A202-20FDEC41EA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F13B90D-5BBC-49D8-B70D-F2657D646E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11760" firstSheet="6" activeTab="13" xr2:uid="{C2B090A9-DA10-49B2-ACF5-02DA27898DB2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" firstSheet="6" activeTab="7" xr2:uid="{C2B090A9-DA10-49B2-ACF5-02DA27898DB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ex78" sheetId="1" r:id="rId1"/>
@@ -1326,7 +1326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1379,6 +1379,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1406,33 +1410,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1519,13 +1496,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1535,6 +1505,13 @@
         <top style="medium">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1554,6 +1531,23 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1570,23 +1564,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1634,13 +1611,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1650,6 +1620,13 @@
         <top style="medium">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1732,13 +1709,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1748,6 +1718,13 @@
         <top style="medium">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1767,6 +1744,24 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1783,24 +1778,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1848,13 +1825,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1864,6 +1834,13 @@
         <top style="medium">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -1961,13 +1938,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1977,6 +1947,13 @@
         <top style="medium">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2057,13 +2034,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2073,6 +2043,13 @@
         <top style="medium">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2210,13 +2187,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2226,6 +2196,13 @@
         <top style="medium">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2242,6 +2219,88 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2270,189 +2329,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2505,7 +2381,61 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2588,6 +2518,53 @@
         </right>
         <top/>
         <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3148,7 +3125,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{98953847-8DE6-4FAB-BDC6-4A7AA0EC4846}" name="Tabela145786911" displayName="Tabela145786911" ref="A3:D33" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="37" tableBorderDxfId="38" totalsRowBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{98953847-8DE6-4FAB-BDC6-4A7AA0EC4846}" name="Tabela145786911" displayName="Tabela145786911" ref="A3:D33" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
   <autoFilter ref="A3:D33" xr:uid="{98953847-8DE6-4FAB-BDC6-4A7AA0EC4846}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{8B855416-14B9-4C92-B193-4BDB798AF7FC}" name="Passo" dataDxfId="35"/>
@@ -3161,21 +3138,21 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{75672EEF-8763-4994-BF28-5A881D6F4450}" name="Tabela145786912" displayName="Tabela145786912" ref="A3:E43" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{75672EEF-8763-4994-BF28-5A881D6F4450}" name="Tabela145786912" displayName="Tabela145786912" ref="A3:E43" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
   <autoFilter ref="A3:E43" xr:uid="{75672EEF-8763-4994-BF28-5A881D6F4450}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{79AF1DF2-4308-486E-8892-24DD4594F5E8}" name="Passo" dataDxfId="27"/>
     <tableColumn id="2" xr3:uid="{679C2F52-C8DD-4858-B49F-ED2A9EB10EFD}" name="valores" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{5E2F27DD-BBEF-4CEC-A7DA-27E59B407A01}" name="novos_valores" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{74CB1271-F6F8-4C2A-BA3A-B1EDC901C9D5}" name="repeticoes" dataDxfId="25"/>
-    <tableColumn id="7" xr3:uid="{39102920-B887-46BB-8534-8F4AAF248CB2}" name="num_selec" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{5E2F27DD-BBEF-4CEC-A7DA-27E59B407A01}" name="novos_valores" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{74CB1271-F6F8-4C2A-BA3A-B1EDC901C9D5}" name="repeticoes" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{39102920-B887-46BB-8534-8F4AAF248CB2}" name="num_selec" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CAEB8896-78D6-4CA6-909A-9F701F9D817A}" name="Tabela14578691113" displayName="Tabela14578691113" ref="A3:C33" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="20" tableBorderDxfId="21" totalsRowBorderDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CAEB8896-78D6-4CA6-909A-9F701F9D817A}" name="Tabela14578691113" displayName="Tabela14578691113" ref="A3:C33" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A3:C33" xr:uid="{CAEB8896-78D6-4CA6-909A-9F701F9D817A}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7A324174-954D-46B2-8F81-7E5C6CCE3ADB}" name="Passo" dataDxfId="18"/>
@@ -3187,20 +3164,20 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6CB782F-DBA2-45D8-ADB8-551F26E2C373}" name="Tabela145786914" displayName="Tabela145786914" ref="A3:D60" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="13" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6CB782F-DBA2-45D8-ADB8-551F26E2C373}" name="Tabela145786914" displayName="Tabela145786914" ref="A3:D60" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="A3:D60" xr:uid="{B6CB782F-DBA2-45D8-ADB8-551F26E2C373}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{12C69BC1-FC46-4C5C-9CDB-12F86B167FC5}" name="Passo" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{C8CFE99A-0C63-45EB-B509-E291E1F7C2F5}" name="valores" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{2F6024E6-95DA-438F-BEAC-9517492B3AF6}" name="x" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{BBBF18F5-322A-469D-86BB-7EFA60F0436C}" name="repetidos" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{2F6024E6-95DA-438F-BEAC-9517492B3AF6}" name="x" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{BBBF18F5-322A-469D-86BB-7EFA60F0436C}" name="repetidos" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{587EC731-1520-405F-A165-EA29ACD77011}" name="Tabela14578691415" displayName="Tabela14578691415" ref="A3:D55" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{587EC731-1520-405F-A165-EA29ACD77011}" name="Tabela14578691415" displayName="Tabela14578691415" ref="A3:D55" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="A3:D55" xr:uid="{587EC731-1520-405F-A165-EA29ACD77011}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1398803E-4539-4837-A401-1E81ACC2B4C9}" name="Passo" dataDxfId="3"/>
@@ -3257,42 +3234,42 @@
   <autoFilter ref="A3:D23" xr:uid="{31185786-3A99-4ADB-90CD-07DCDA33DA5B}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{02708C67-653A-435A-AE8E-4276712282E7}" name="Passo" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{2ACAC51E-EF90-48E2-A867-8303A93BBBEA}" name="A" dataDxfId="61"/>
-    <tableColumn id="4" xr3:uid="{3B792624-EB18-4C37-B597-259466842F9D}" name="num" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{C0B5AB72-A596-4E03-B8D5-9C8D648172C5}" name="M" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{2ACAC51E-EF90-48E2-A867-8303A93BBBEA}" name="A" dataDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{3B792624-EB18-4C37-B597-259466842F9D}" name="num" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{C0B5AB72-A596-4E03-B8D5-9C8D648172C5}" name="M" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BE70E156-EE5F-4CB4-B53F-B168EDB5C595}" name="Tabela14578" displayName="Tabela14578" ref="A3:C34" totalsRowShown="0" headerRowDxfId="76" headerRowBorderDxfId="75" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BE70E156-EE5F-4CB4-B53F-B168EDB5C595}" name="Tabela14578" displayName="Tabela14578" ref="A3:C34" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
   <autoFilter ref="A3:C34" xr:uid="{BE70E156-EE5F-4CB4-B53F-B168EDB5C595}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D2055CA2-DD2A-47AA-B604-5F44BD53352B}" name="Passo" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{59DF4C3B-C256-42B5-B08A-0FE461381D6D}" name="vetor" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{77BB9EC1-7F05-4762-A51E-5E0327A9462C}" name="temporario" dataDxfId="58"/>
+    <tableColumn id="1" xr3:uid="{D2055CA2-DD2A-47AA-B604-5F44BD53352B}" name="Passo" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{59DF4C3B-C256-42B5-B08A-0FE461381D6D}" name="vetor" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{77BB9EC1-7F05-4762-A51E-5E0327A9462C}" name="temporario" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4E39FD7B-1391-40FC-B115-2400EDF67D52}" name="Tabela1457810" displayName="Tabela1457810" ref="A3:E14" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62" headerRowBorderDxfId="70" tableBorderDxfId="69" totalsRowBorderDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4E39FD7B-1391-40FC-B115-2400EDF67D52}" name="Tabela1457810" displayName="Tabela1457810" ref="A3:E14" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
   <autoFilter ref="A3:E14" xr:uid="{4E39FD7B-1391-40FC-B115-2400EDF67D52}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AB3D9FE7-8ACD-4511-A1E2-63DF42F241A5}" name="Passo" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{53C1919E-04CD-4EA7-A99B-94E1E09BD7A5}" name="num_vetor" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{7C101053-61DE-4A9D-AC4C-94797AFC6395}" name="A" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{0977DE1E-9BEB-4F74-BC4A-8C7B26119473}" name="B" dataDxfId="65"/>
-    <tableColumn id="4" xr3:uid="{0B3A4F6A-5705-43DE-90F0-8E8B0646D72D}" name="Soma" dataDxfId="64"/>
+    <tableColumn id="1" xr3:uid="{AB3D9FE7-8ACD-4511-A1E2-63DF42F241A5}" name="Passo" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{53C1919E-04CD-4EA7-A99B-94E1E09BD7A5}" name="num_vetor" dataDxfId="60"/>
+    <tableColumn id="2" xr3:uid="{7C101053-61DE-4A9D-AC4C-94797AFC6395}" name="A" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{0977DE1E-9BEB-4F74-BC4A-8C7B26119473}" name="B" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{0B3A4F6A-5705-43DE-90F0-8E8B0646D72D}" name="Soma" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B22B2C47-2A5B-4F41-BE1C-79DFCAC8E14C}" name="Tabela145786" displayName="Tabela145786" ref="A3:F23" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="54" tableBorderDxfId="55" totalsRowBorderDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B22B2C47-2A5B-4F41-BE1C-79DFCAC8E14C}" name="Tabela145786" displayName="Tabela145786" ref="A3:F23" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
   <autoFilter ref="A3:F23" xr:uid="{B22B2C47-2A5B-4F41-BE1C-79DFCAC8E14C}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{3AB2A6DB-3791-4A40-8E7D-583AB25EA1D2}" name="Passo" dataDxfId="52"/>
@@ -3307,7 +3284,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C42FBFD-38BB-48E3-B014-112ECB6EC4B8}" name="Tabela1457869" displayName="Tabela1457869" ref="A3:C23" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="44" tableBorderDxfId="45" totalsRowBorderDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C42FBFD-38BB-48E3-B014-112ECB6EC4B8}" name="Tabela1457869" displayName="Tabela1457869" ref="A3:C23" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
   <autoFilter ref="A3:C23" xr:uid="{0C42FBFD-38BB-48E3-B014-112ECB6EC4B8}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{CFF4CCBD-E6C8-4BC0-866D-689AA05BF46B}" name="Passo" dataDxfId="42"/>
@@ -3632,18 +3609,18 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
     </row>
     <row r="3" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
@@ -3936,20 +3913,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="34"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="34"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4357,18 +4334,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -4979,7 +4956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA8C1589-10F0-4D23-B4E3-5B990AE82D01}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -4992,18 +4969,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="34"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -5316,30 +5293,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC9DAFD-F507-4E38-81EB-57B74C6F0D2B}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -6078,7 +6056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD30514-7204-46FB-A86A-E352836414B9}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
@@ -6091,18 +6069,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -6860,20 +6838,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -7533,18 +7511,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -8162,18 +8140,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -8791,18 +8769,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -9106,18 +9084,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="34"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="34"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -9499,222 +9477,222 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="8" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
+      <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="9">
         <v>4</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30">
-        <v>2</v>
-      </c>
-      <c r="B5" s="32">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9">
         <v>4</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+      <c r="A6" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="9">
         <v>4</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="30">
+      <c r="A7" s="7">
         <v>4</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="30">
+      <c r="A8" s="7">
         <v>5</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="9">
         <v>4</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="32" t="s">
+      <c r="E8" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="30">
+      <c r="A9" s="7">
         <v>6</v>
       </c>
-      <c r="B9" s="32">
+      <c r="B9" s="9">
         <v>4</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="32" t="s">
+      <c r="D9" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+      <c r="A10" s="7">
         <v>7</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D10" s="32" t="s">
+      <c r="D10" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="30">
+      <c r="A11" s="7">
         <v>8</v>
       </c>
-      <c r="B11" s="32">
+      <c r="B11" s="9">
         <v>4</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="9" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="30">
+      <c r="A12" s="7">
         <v>9</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="9">
         <v>4</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E12" s="32" t="s">
+      <c r="E12" s="9" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="30">
+      <c r="A13" s="7">
         <v>10</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="9">
         <v>4</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="9" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="30">
+      <c r="A14" s="7">
         <v>11</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="9">
         <v>4</v>
       </c>
-      <c r="C14" s="31" t="s">
+      <c r="C14" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="32" t="s">
+      <c r="D14" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="9" t="s">
         <v>140</v>
       </c>
     </row>
@@ -9731,41 +9709,41 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CDC1CC1-FF96-473D-A456-7979CE8F139C}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>14</v>
       </c>
@@ -9784,12 +9762,8 @@
       <c r="F3" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
@@ -9808,12 +9782,8 @@
       <c r="F4" s="3">
         <v>0</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
@@ -9832,12 +9802,8 @@
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>3</v>
       </c>
@@ -9857,7 +9823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>4</v>
       </c>
@@ -9877,7 +9843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>5</v>
       </c>
@@ -9897,7 +9863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>6</v>
       </c>
@@ -9917,7 +9883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>7</v>
       </c>
@@ -9937,7 +9903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8</v>
       </c>
@@ -9957,7 +9923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>9</v>
       </c>
@@ -9977,7 +9943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>10</v>
       </c>
@@ -9997,7 +9963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>11</v>
       </c>
@@ -10017,7 +9983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>12</v>
       </c>
@@ -10037,7 +10003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>13</v>
       </c>
@@ -10198,14 +10164,14 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10237,22 +10203,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">

</xml_diff>

<commit_message>
Adicionando teste de mesa do ex 77 e finalizando todas as atividades.
</commit_message>
<xml_diff>
--- a/TestesMesa/Testes_de_Mesa.xlsx
+++ b/TestesMesa/Testes_de_Mesa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Just Coding\JAVA\FATEC\LP1\TestesMesa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1843A719-D865-44A2-9084-00342377A193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6C153E-D2B9-4BB2-B8CF-E3EE099063F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C2B090A9-DA10-49B2-ACF5-02DA27898DB2}"/>
+    <workbookView xWindow="-15480" yWindow="-120" windowWidth="15600" windowHeight="11760" xr2:uid="{C2B090A9-DA10-49B2-ACF5-02DA27898DB2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ex77" sheetId="15" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="354">
   <si>
     <t>nomes</t>
   </si>
@@ -1082,6 +1082,36 @@
   </si>
   <si>
     <t>Exercicio 91</t>
+  </si>
+  <si>
+    <t>Exercicio 77</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>aux</t>
+  </si>
+  <si>
+    <t>[5,1,4,2,7,8,3,6]</t>
+  </si>
+  <si>
+    <t>[6,1,4,2,7,8,3,1]</t>
+  </si>
+  <si>
+    <t>[6,3,4,2,7,8,4,1]</t>
+  </si>
+  <si>
+    <t>[6,3,8,2,7,2,4,1]</t>
+  </si>
+  <si>
+    <t>[6,3,8,7,7,2,4,1]</t>
+  </si>
+  <si>
+    <t>[6,3,6,7,7,2,4,1]</t>
+  </si>
+  <si>
+    <t>[6,3,6,7,7,2,7,1]</t>
   </si>
 </sst>
 </file>
@@ -1327,7 +1357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1411,11 +1441,130 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="115">
+  <dxfs count="122">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -3113,184 +3262,196 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{181A0719-1EE9-4776-939A-DD4A1F248B4A}" name="Tabela1" displayName="Tabela1" ref="B4:E23" totalsRowShown="0" headerRowDxfId="114" headerRowBorderDxfId="113" tableBorderDxfId="112" totalsRowBorderDxfId="111">
-  <autoFilter ref="B4:E23" xr:uid="{181A0719-1EE9-4776-939A-DD4A1F248B4A}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{0D7E30CA-28FF-4DFD-BA81-E7F9D24DB814}" name="Passo" dataDxfId="110"/>
-    <tableColumn id="2" xr3:uid="{4C3B8BEB-F00B-41EA-92E0-220856B93104}" name="nomes" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{2332C368-92DB-46FC-AC5E-13C1B246CA5B}" name="pessoa" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{54C8FF23-2140-454C-A6C9-52C0C604D370}" name="encontra" dataDxfId="107"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{08236354-32F3-4CA2-9F5F-B81D72550776}" name="Tabela14516" displayName="Tabela14516" ref="A3:C10" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="4" tableBorderDxfId="5" totalsRowBorderDxfId="3">
+  <autoFilter ref="A3:C10" xr:uid="{08236354-32F3-4CA2-9F5F-B81D72550776}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{8B2BD827-9EE6-48E2-B278-CA20F5D9AE02}" name="Passo" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E079C2C6-96E4-4C72-8FD0-BE0E19C5D1FC}" name="v" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{0BBD0672-91E4-4060-9144-C0EFB34F7F67}" name="aux" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{98953847-8DE6-4FAB-BDC6-4A7AA0EC4846}" name="Tabela145786911" displayName="Tabela145786911" ref="A3:D33" totalsRowShown="0" headerRowDxfId="39" headerRowBorderDxfId="38" tableBorderDxfId="37" totalsRowBorderDxfId="36">
-  <autoFilter ref="A3:D33" xr:uid="{98953847-8DE6-4FAB-BDC6-4A7AA0EC4846}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8B855416-14B9-4C92-B193-4BDB798AF7FC}" name="Passo" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{362D1E7F-4DAD-43EE-9DF2-A9DD35467323}" name="valores" dataDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{CB77369F-F11F-43DF-B041-5D38307EDE19}" name="novos_valores" dataDxfId="33"/>
-    <tableColumn id="3" xr3:uid="{05CC0BC4-46B4-4362-A4ED-C82499997286}" name="temporario" dataDxfId="32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C42FBFD-38BB-48E3-B014-112ECB6EC4B8}" name="Tabela1457869" displayName="Tabela1457869" ref="A3:C23" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51" totalsRowBorderDxfId="50">
+  <autoFilter ref="A3:C23" xr:uid="{0C42FBFD-38BB-48E3-B014-112ECB6EC4B8}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{CFF4CCBD-E6C8-4BC0-866D-689AA05BF46B}" name="Passo" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{CCE6B4DE-8B4B-45E7-B117-1817C7612A7E}" name="valores" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{44FF75F1-38D3-47C4-90A4-DCD45C3A3EC1}" name="temporario" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{75672EEF-8763-4994-BF28-5A881D6F4450}" name="Tabela145786912" displayName="Tabela145786912" ref="A3:E43" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30" tableBorderDxfId="29" totalsRowBorderDxfId="28">
-  <autoFilter ref="A3:E43" xr:uid="{75672EEF-8763-4994-BF28-5A881D6F4450}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{79AF1DF2-4308-486E-8892-24DD4594F5E8}" name="Passo" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{679C2F52-C8DD-4858-B49F-ED2A9EB10EFD}" name="valores" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{5E2F27DD-BBEF-4CEC-A7DA-27E59B407A01}" name="novos_valores" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{74CB1271-F6F8-4C2A-BA3A-B1EDC901C9D5}" name="repeticoes" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{39102920-B887-46BB-8534-8F4AAF248CB2}" name="num_selec" dataDxfId="23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{98953847-8DE6-4FAB-BDC6-4A7AA0EC4846}" name="Tabela145786911" displayName="Tabela145786911" ref="A3:D33" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
+  <autoFilter ref="A3:D33" xr:uid="{98953847-8DE6-4FAB-BDC6-4A7AA0EC4846}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8B855416-14B9-4C92-B193-4BDB798AF7FC}" name="Passo" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{362D1E7F-4DAD-43EE-9DF2-A9DD35467323}" name="valores" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{CB77369F-F11F-43DF-B041-5D38307EDE19}" name="novos_valores" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{05CC0BC4-46B4-4362-A4ED-C82499997286}" name="temporario" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CAEB8896-78D6-4CA6-909A-9F701F9D817A}" name="Tabela14578691113" displayName="Tabela14578691113" ref="A3:C33" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
-  <autoFilter ref="A3:C33" xr:uid="{CAEB8896-78D6-4CA6-909A-9F701F9D817A}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{7A324174-954D-46B2-8F81-7E5C6CCE3ADB}" name="Passo" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{38E81113-07C3-4269-A7DB-5EE63ACE8E01}" name="V1" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{79376356-236B-4E20-AF41-580414B910F4}" name="V2" dataDxfId="16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{75672EEF-8763-4994-BF28-5A881D6F4450}" name="Tabela145786912" displayName="Tabela145786912" ref="A3:E43" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
+  <autoFilter ref="A3:E43" xr:uid="{75672EEF-8763-4994-BF28-5A881D6F4450}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{79AF1DF2-4308-486E-8892-24DD4594F5E8}" name="Passo" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{679C2F52-C8DD-4858-B49F-ED2A9EB10EFD}" name="valores" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{5E2F27DD-BBEF-4CEC-A7DA-27E59B407A01}" name="novos_valores" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{74CB1271-F6F8-4C2A-BA3A-B1EDC901C9D5}" name="repeticoes" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{39102920-B887-46BB-8534-8F4AAF248CB2}" name="num_selec" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6CB782F-DBA2-45D8-ADB8-551F26E2C373}" name="Tabela145786914" displayName="Tabela145786914" ref="A3:D60" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
-  <autoFilter ref="A3:D60" xr:uid="{B6CB782F-DBA2-45D8-ADB8-551F26E2C373}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{12C69BC1-FC46-4C5C-9CDB-12F86B167FC5}" name="Passo" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C8CFE99A-0C63-45EB-B509-E291E1F7C2F5}" name="valores" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{2F6024E6-95DA-438F-BEAC-9517492B3AF6}" name="x" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{BBBF18F5-322A-469D-86BB-7EFA60F0436C}" name="repetidos" dataDxfId="8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{CAEB8896-78D6-4CA6-909A-9F701F9D817A}" name="Tabela14578691113" displayName="Tabela14578691113" ref="A3:C33" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27" totalsRowBorderDxfId="26">
+  <autoFilter ref="A3:C33" xr:uid="{CAEB8896-78D6-4CA6-909A-9F701F9D817A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{7A324174-954D-46B2-8F81-7E5C6CCE3ADB}" name="Passo" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{38E81113-07C3-4269-A7DB-5EE63ACE8E01}" name="V1" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{79376356-236B-4E20-AF41-580414B910F4}" name="V2" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{587EC731-1520-405F-A165-EA29ACD77011}" name="Tabela14578691415" displayName="Tabela14578691415" ref="A3:D55" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="6" tableBorderDxfId="5" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{B6CB782F-DBA2-45D8-ADB8-551F26E2C373}" name="Tabela145786914" displayName="Tabela145786914" ref="A3:D60" totalsRowShown="0" headerRowDxfId="22" headerRowBorderDxfId="21" tableBorderDxfId="20" totalsRowBorderDxfId="19">
+  <autoFilter ref="A3:D60" xr:uid="{B6CB782F-DBA2-45D8-ADB8-551F26E2C373}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{12C69BC1-FC46-4C5C-9CDB-12F86B167FC5}" name="Passo" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{C8CFE99A-0C63-45EB-B509-E291E1F7C2F5}" name="valores" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{2F6024E6-95DA-438F-BEAC-9517492B3AF6}" name="x" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{BBBF18F5-322A-469D-86BB-7EFA60F0436C}" name="repetidos" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{587EC731-1520-405F-A165-EA29ACD77011}" name="Tabela14578691415" displayName="Tabela14578691415" ref="A3:D55" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A3:D55" xr:uid="{587EC731-1520-405F-A165-EA29ACD77011}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1398803E-4539-4837-A401-1E81ACC2B4C9}" name="Passo" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{B165A451-8B68-4CE8-BC01-3AF0CE69CB5E}" name="VET" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{A9FB9D35-B291-4B71-8CD2-A7FDA12CEDF8}" name="numero_repetir" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{72B6D4CC-5E4E-417E-AFCF-E98D25FE0702}" name="conta" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{1398803E-4539-4837-A401-1E81ACC2B4C9}" name="Passo" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B165A451-8B68-4CE8-BC01-3AF0CE69CB5E}" name="VET" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{A9FB9D35-B291-4B71-8CD2-A7FDA12CEDF8}" name="numero_repetir" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{72B6D4CC-5E4E-417E-AFCF-E98D25FE0702}" name="conta" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{503352B8-EA3F-4B09-A19D-3FD323FD45ED}" name="Tabela13" displayName="Tabela13" ref="A3:E44" totalsRowShown="0" headerRowDxfId="106" headerRowBorderDxfId="105" tableBorderDxfId="104" totalsRowBorderDxfId="103">
-  <autoFilter ref="A3:E44" xr:uid="{503352B8-EA3F-4B09-A19D-3FD323FD45ED}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C79ABD21-DBCE-4E44-BCD8-E1DF443DA06B}" name="Passo" dataDxfId="102"/>
-    <tableColumn id="2" xr3:uid="{83422539-6CAE-49E9-9901-E1AD6254C118}" name="notas" dataDxfId="101"/>
-    <tableColumn id="3" xr3:uid="{B3E536A7-A678-452F-9787-CF051047BB83}" name="total" dataDxfId="100"/>
-    <tableColumn id="4" xr3:uid="{7CB17B6C-26B5-49D7-9169-1D464901C5A2}" name="media" dataDxfId="99"/>
-    <tableColumn id="5" xr3:uid="{13C39996-2E2C-495F-8375-298191C62758}" name="acima" dataDxfId="98"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{181A0719-1EE9-4776-939A-DD4A1F248B4A}" name="Tabela1" displayName="Tabela1" ref="B4:E23" totalsRowShown="0" headerRowDxfId="121" headerRowBorderDxfId="120" tableBorderDxfId="119" totalsRowBorderDxfId="118">
+  <autoFilter ref="B4:E23" xr:uid="{181A0719-1EE9-4776-939A-DD4A1F248B4A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{0D7E30CA-28FF-4DFD-BA81-E7F9D24DB814}" name="Passo" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{4C3B8BEB-F00B-41EA-92E0-220856B93104}" name="nomes" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{2332C368-92DB-46FC-AC5E-13C1B246CA5B}" name="pessoa" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{54C8FF23-2140-454C-A6C9-52C0C604D370}" name="encontra" dataDxfId="114"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F4D5731-7C13-48A4-A20A-56174D43EE44}" name="Tabela14" displayName="Tabela14" ref="A3:D44" totalsRowShown="0" headerRowDxfId="97" headerRowBorderDxfId="96" tableBorderDxfId="95" totalsRowBorderDxfId="94">
-  <autoFilter ref="A3:D44" xr:uid="{6F4D5731-7C13-48A4-A20A-56174D43EE44}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{06BC8F5A-6E66-442F-88FB-8A6433890BB9}" name="Passo" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{B3614919-970E-4B43-8A1D-00578305CDAC}" name="Q" dataDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{CAEEB636-1E6A-49E5-8776-86EEC75E2971}" name="pos" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{0DD38BE3-1076-4881-994E-1009FAD78C7C}" name="maior" dataDxfId="90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{503352B8-EA3F-4B09-A19D-3FD323FD45ED}" name="Tabela13" displayName="Tabela13" ref="A3:E44" totalsRowShown="0" headerRowDxfId="113" headerRowBorderDxfId="112" tableBorderDxfId="111" totalsRowBorderDxfId="110">
+  <autoFilter ref="A3:E44" xr:uid="{503352B8-EA3F-4B09-A19D-3FD323FD45ED}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{C79ABD21-DBCE-4E44-BCD8-E1DF443DA06B}" name="Passo" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{83422539-6CAE-49E9-9901-E1AD6254C118}" name="notas" dataDxfId="108"/>
+    <tableColumn id="3" xr3:uid="{B3E536A7-A678-452F-9787-CF051047BB83}" name="total" dataDxfId="107"/>
+    <tableColumn id="4" xr3:uid="{7CB17B6C-26B5-49D7-9169-1D464901C5A2}" name="media" dataDxfId="106"/>
+    <tableColumn id="5" xr3:uid="{13C39996-2E2C-495F-8375-298191C62758}" name="acima" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DCBA3F8D-7C94-48BF-B149-23ADCC54720E}" name="Tabela145" displayName="Tabela145" ref="A3:D44" totalsRowShown="0" headerRowDxfId="89" headerRowBorderDxfId="88" tableBorderDxfId="87" totalsRowBorderDxfId="86">
-  <autoFilter ref="A3:D44" xr:uid="{DCBA3F8D-7C94-48BF-B149-23ADCC54720E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{6F4D5731-7C13-48A4-A20A-56174D43EE44}" name="Tabela14" displayName="Tabela14" ref="A3:D44" totalsRowShown="0" headerRowDxfId="104" headerRowBorderDxfId="103" tableBorderDxfId="102" totalsRowBorderDxfId="101">
+  <autoFilter ref="A3:D44" xr:uid="{6F4D5731-7C13-48A4-A20A-56174D43EE44}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{25E3DA19-8A44-4886-8D0B-811B48B7244D}" name="Passo" dataDxfId="85"/>
-    <tableColumn id="2" xr3:uid="{8B7EDF9A-526D-45B8-A281-D23F9747DF3F}" name="Q" dataDxfId="84"/>
-    <tableColumn id="3" xr3:uid="{C14511EF-BF06-4E85-AB64-7BA4C566551A}" name="pos" dataDxfId="83"/>
-    <tableColumn id="4" xr3:uid="{2EB256CF-FD74-4D7F-B86C-2B3A5AD1534B}" name="menor" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{06BC8F5A-6E66-442F-88FB-8A6433890BB9}" name="Passo" dataDxfId="100"/>
+    <tableColumn id="2" xr3:uid="{B3614919-970E-4B43-8A1D-00578305CDAC}" name="Q" dataDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{CAEEB636-1E6A-49E5-8776-86EEC75E2971}" name="pos" dataDxfId="98"/>
+    <tableColumn id="4" xr3:uid="{0DD38BE3-1076-4881-994E-1009FAD78C7C}" name="maior" dataDxfId="97"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{31185786-3A99-4ADB-90CD-07DCDA33DA5B}" name="Tabela1457" displayName="Tabela1457" ref="A3:D23" totalsRowShown="0" headerRowDxfId="81" headerRowBorderDxfId="80" tableBorderDxfId="79" totalsRowBorderDxfId="78">
-  <autoFilter ref="A3:D23" xr:uid="{31185786-3A99-4ADB-90CD-07DCDA33DA5B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DCBA3F8D-7C94-48BF-B149-23ADCC54720E}" name="Tabela145" displayName="Tabela145" ref="A3:D44" totalsRowShown="0" headerRowDxfId="96" headerRowBorderDxfId="95" tableBorderDxfId="94" totalsRowBorderDxfId="93">
+  <autoFilter ref="A3:D44" xr:uid="{DCBA3F8D-7C94-48BF-B149-23ADCC54720E}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{02708C67-653A-435A-AE8E-4276712282E7}" name="Passo" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{2ACAC51E-EF90-48E2-A867-8303A93BBBEA}" name="A" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{3B792624-EB18-4C37-B597-259466842F9D}" name="num" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{C0B5AB72-A596-4E03-B8D5-9C8D648172C5}" name="M" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{25E3DA19-8A44-4886-8D0B-811B48B7244D}" name="Passo" dataDxfId="92"/>
+    <tableColumn id="2" xr3:uid="{8B7EDF9A-526D-45B8-A281-D23F9747DF3F}" name="Q" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{C14511EF-BF06-4E85-AB64-7BA4C566551A}" name="pos" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{2EB256CF-FD74-4D7F-B86C-2B3A5AD1534B}" name="menor" dataDxfId="89"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BE70E156-EE5F-4CB4-B53F-B168EDB5C595}" name="Tabela14578" displayName="Tabela14578" ref="A3:C34" totalsRowShown="0" headerRowDxfId="73" headerRowBorderDxfId="72" tableBorderDxfId="71" totalsRowBorderDxfId="70">
-  <autoFilter ref="A3:C34" xr:uid="{BE70E156-EE5F-4CB4-B53F-B168EDB5C595}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D2055CA2-DD2A-47AA-B604-5F44BD53352B}" name="Passo" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{59DF4C3B-C256-42B5-B08A-0FE461381D6D}" name="vetor" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{77BB9EC1-7F05-4762-A51E-5E0327A9462C}" name="temporario" dataDxfId="67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{31185786-3A99-4ADB-90CD-07DCDA33DA5B}" name="Tabela1457" displayName="Tabela1457" ref="A3:D23" totalsRowShown="0" headerRowDxfId="88" headerRowBorderDxfId="87" tableBorderDxfId="86" totalsRowBorderDxfId="85">
+  <autoFilter ref="A3:D23" xr:uid="{31185786-3A99-4ADB-90CD-07DCDA33DA5B}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{02708C67-653A-435A-AE8E-4276712282E7}" name="Passo" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{2ACAC51E-EF90-48E2-A867-8303A93BBBEA}" name="A" dataDxfId="83"/>
+    <tableColumn id="4" xr3:uid="{3B792624-EB18-4C37-B597-259466842F9D}" name="num" dataDxfId="82"/>
+    <tableColumn id="3" xr3:uid="{C0B5AB72-A596-4E03-B8D5-9C8D648172C5}" name="M" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4E39FD7B-1391-40FC-B115-2400EDF67D52}" name="Tabela1457810" displayName="Tabela1457810" ref="A3:E14" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
-  <autoFilter ref="A3:E14" xr:uid="{4E39FD7B-1391-40FC-B115-2400EDF67D52}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AB3D9FE7-8ACD-4511-A1E2-63DF42F241A5}" name="Passo" dataDxfId="61"/>
-    <tableColumn id="5" xr3:uid="{53C1919E-04CD-4EA7-A99B-94E1E09BD7A5}" name="num_vetor" dataDxfId="60"/>
-    <tableColumn id="2" xr3:uid="{7C101053-61DE-4A9D-AC4C-94797AFC6395}" name="A" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{0977DE1E-9BEB-4F74-BC4A-8C7B26119473}" name="B" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{0B3A4F6A-5705-43DE-90F0-8E8B0646D72D}" name="Soma" dataDxfId="57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BE70E156-EE5F-4CB4-B53F-B168EDB5C595}" name="Tabela14578" displayName="Tabela14578" ref="A3:C34" totalsRowShown="0" headerRowDxfId="80" headerRowBorderDxfId="79" tableBorderDxfId="78" totalsRowBorderDxfId="77">
+  <autoFilter ref="A3:C34" xr:uid="{BE70E156-EE5F-4CB4-B53F-B168EDB5C595}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{D2055CA2-DD2A-47AA-B604-5F44BD53352B}" name="Passo" dataDxfId="76"/>
+    <tableColumn id="2" xr3:uid="{59DF4C3B-C256-42B5-B08A-0FE461381D6D}" name="vetor" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{77BB9EC1-7F05-4762-A51E-5E0327A9462C}" name="temporario" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B22B2C47-2A5B-4F41-BE1C-79DFCAC8E14C}" name="Tabela145786" displayName="Tabela145786" ref="A3:F23" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54" totalsRowBorderDxfId="53">
-  <autoFilter ref="A3:F23" xr:uid="{B22B2C47-2A5B-4F41-BE1C-79DFCAC8E14C}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{3AB2A6DB-3791-4A40-8E7D-583AB25EA1D2}" name="Passo" dataDxfId="52"/>
-    <tableColumn id="2" xr3:uid="{59F7E7F5-206F-4F02-B52E-EA5CDB507E0E}" name="temperaturas" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{40354B2D-43A6-43DF-86C8-D2DF1CE7013F}" name="menor_temp" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{E0EA673A-452F-4536-9509-6A5F78D2A9BF}" name="maior_temp" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{A1D740E6-5223-4C2B-9BE6-4B62BDCB79CF}" name="media" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{C0E3C075-577D-4077-803B-C25936DC3074}" name="num_dias" dataDxfId="47"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4E39FD7B-1391-40FC-B115-2400EDF67D52}" name="Tabela1457810" displayName="Tabela1457810" ref="A3:E14" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
+  <autoFilter ref="A3:E14" xr:uid="{4E39FD7B-1391-40FC-B115-2400EDF67D52}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{AB3D9FE7-8ACD-4511-A1E2-63DF42F241A5}" name="Passo" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{53C1919E-04CD-4EA7-A99B-94E1E09BD7A5}" name="num_vetor" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{7C101053-61DE-4A9D-AC4C-94797AFC6395}" name="A" dataDxfId="66"/>
+    <tableColumn id="3" xr3:uid="{0977DE1E-9BEB-4F74-BC4A-8C7B26119473}" name="B" dataDxfId="65"/>
+    <tableColumn id="4" xr3:uid="{0B3A4F6A-5705-43DE-90F0-8E8B0646D72D}" name="Soma" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0C42FBFD-38BB-48E3-B014-112ECB6EC4B8}" name="Tabela1457869" displayName="Tabela1457869" ref="A3:C23" totalsRowShown="0" headerRowDxfId="46" headerRowBorderDxfId="45" tableBorderDxfId="44" totalsRowBorderDxfId="43">
-  <autoFilter ref="A3:C23" xr:uid="{0C42FBFD-38BB-48E3-B014-112ECB6EC4B8}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CFF4CCBD-E6C8-4BC0-866D-689AA05BF46B}" name="Passo" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{CCE6B4DE-8B4B-45E7-B117-1817C7612A7E}" name="valores" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{44FF75F1-38D3-47C4-90A4-DCD45C3A3EC1}" name="temporario" dataDxfId="40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{B22B2C47-2A5B-4F41-BE1C-79DFCAC8E14C}" name="Tabela145786" displayName="Tabela145786" ref="A3:F23" totalsRowShown="0" headerRowDxfId="63" headerRowBorderDxfId="62" tableBorderDxfId="61" totalsRowBorderDxfId="60">
+  <autoFilter ref="A3:F23" xr:uid="{B22B2C47-2A5B-4F41-BE1C-79DFCAC8E14C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{3AB2A6DB-3791-4A40-8E7D-583AB25EA1D2}" name="Passo" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{59F7E7F5-206F-4F02-B52E-EA5CDB507E0E}" name="temperaturas" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{40354B2D-43A6-43DF-86C8-D2DF1CE7013F}" name="menor_temp" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{E0EA673A-452F-4536-9509-6A5F78D2A9BF}" name="maior_temp" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{A1D740E6-5223-4C2B-9BE6-4B62BDCB79CF}" name="media" dataDxfId="55"/>
+    <tableColumn id="6" xr3:uid="{C0E3C075-577D-4077-803B-C25936DC3074}" name="num_dias" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3593,13 +3754,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68F8852A-AF4F-46F2-9785-6BA84D57EFD9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="32"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C7" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C10" s="3">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C2"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -6810,8 +7086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06870014-0999-4B69-BB91-09085D1A8B1F}">
   <dimension ref="B1:E23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8418,8 +8694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589973D7-74EE-4B69-AA8D-5E171D1C0D1E}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection sqref="A1:D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>